<commit_message>
add text rule and fix
</commit_message>
<xml_diff>
--- a/venv/eyesexamgame/config.xlsx
+++ b/venv/eyesexamgame/config.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="level" sheetId="1" r:id="rId1"/>
+    <sheet name="sentence" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="37">
   <si>
     <t>display_time</t>
   </si>
@@ -31,59 +32,125 @@
     <t>is_random</t>
   </si>
   <si>
+    <t>plus_num</t>
+  </si>
+  <si>
+    <t>grid_picture</t>
+  </si>
+  <si>
+    <t>grid_picture_clicked</t>
+  </si>
+  <si>
+    <t>font_color</t>
+  </si>
+  <si>
+    <t>font_type</t>
+  </si>
+  <si>
+    <t>font_size</t>
+  </si>
+  <si>
+    <t>level_id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>level_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>num</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grid.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grid.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>grid_click.png</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55,221,14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>55,221,14</t>
+  </si>
+  <si>
+    <t>id</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>content</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>分组</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type=2时，取的sentence表中最大index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>type=2时，取的sentence表中最小index</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>random_min</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>random_max</t>
-  </si>
-  <si>
-    <t>plus_num</t>
-  </si>
-  <si>
-    <t>grid_picture</t>
-  </si>
-  <si>
-    <t>grid_picture_clicked</t>
-  </si>
-  <si>
-    <t>font_color</t>
-  </si>
-  <si>
-    <t>font_type</t>
-  </si>
-  <si>
-    <t>font_size</t>
-  </si>
-  <si>
-    <t>level_id</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>level_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>num</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grid.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grid.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>grid_click.png</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>55,221,14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>55,221,14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SimHei</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寻寻觅觅</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>冷冷清清</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>凄凄惨惨戚戚</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>乍暖还寒时候</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最难将息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>三杯两盏淡酒</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>怎敌他晚来风急</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雁过也正伤心</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -126,8 +193,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -429,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:P12"/>
+  <dimension ref="A1:P12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -444,7 +514,8 @@
     <col min="5" max="5" width="5.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="8.5" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.75" customWidth="1"/>
+    <col min="10" max="10" width="11.5" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="13.875" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22.75" bestFit="1" customWidth="1"/>
@@ -452,12 +523,20 @@
     <col min="15" max="16" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:16" s="1" customFormat="1" ht="54" x14ac:dyDescent="0.15">
+      <c r="I1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -469,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>3</v>
@@ -478,28 +557,28 @@
         <v>4</v>
       </c>
       <c r="I2" t="s">
+        <v>26</v>
+      </c>
+      <c r="J2" t="s">
+        <v>27</v>
+      </c>
+      <c r="K2" t="s">
         <v>5</v>
       </c>
-      <c r="J2" t="s">
+      <c r="L2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
         <v>7</v>
       </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" t="s">
         <v>9</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>10</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.15">
@@ -507,7 +586,7 @@
         <v>1</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -528,25 +607,28 @@
         <v>0</v>
       </c>
       <c r="I3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K3">
         <v>1</v>
       </c>
       <c r="L3" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" t="s">
         <v>16</v>
       </c>
-      <c r="M3" t="s">
-        <v>18</v>
-      </c>
       <c r="N3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+      <c r="O3" t="s">
+        <v>28</v>
       </c>
       <c r="P3">
-        <v>80</v>
+        <v>60</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.15">
@@ -554,7 +636,7 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4">
         <v>3</v>
@@ -575,22 +657,25 @@
         <v>0</v>
       </c>
       <c r="I4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K4">
         <v>1</v>
       </c>
       <c r="L4" t="s">
+        <v>15</v>
+      </c>
+      <c r="M4" t="s">
+        <v>16</v>
+      </c>
+      <c r="N4" t="s">
         <v>17</v>
       </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
-      <c r="N4" t="s">
-        <v>19</v>
+      <c r="O4" t="s">
+        <v>28</v>
       </c>
       <c r="P4">
         <v>80</v>
@@ -601,7 +686,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C5">
         <v>5</v>
@@ -622,22 +707,25 @@
         <v>0</v>
       </c>
       <c r="I5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
         <v>16</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>18</v>
       </c>
-      <c r="N5" t="s">
-        <v>20</v>
+      <c r="O5" t="s">
+        <v>28</v>
       </c>
       <c r="P5">
         <v>80</v>
@@ -678,13 +766,13 @@
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N6" t="s">
         <v>18</v>
-      </c>
-      <c r="N6" t="s">
-        <v>20</v>
       </c>
       <c r="P6">
         <v>80</v>
@@ -725,13 +813,13 @@
         <v>1</v>
       </c>
       <c r="L7" t="s">
+        <v>14</v>
+      </c>
+      <c r="M7" t="s">
         <v>16</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>18</v>
-      </c>
-      <c r="N7" t="s">
-        <v>20</v>
       </c>
       <c r="P7">
         <v>80</v>
@@ -772,13 +860,13 @@
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M8" t="s">
+        <v>16</v>
+      </c>
+      <c r="N8" t="s">
         <v>18</v>
-      </c>
-      <c r="N8" t="s">
-        <v>20</v>
       </c>
       <c r="P8">
         <v>80</v>
@@ -819,13 +907,13 @@
         <v>1</v>
       </c>
       <c r="L9" t="s">
+        <v>14</v>
+      </c>
+      <c r="M9" t="s">
         <v>16</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>18</v>
-      </c>
-      <c r="N9" t="s">
-        <v>20</v>
       </c>
       <c r="P9">
         <v>80</v>
@@ -866,13 +954,13 @@
         <v>1</v>
       </c>
       <c r="L10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M10" t="s">
+        <v>16</v>
+      </c>
+      <c r="N10" t="s">
         <v>18</v>
-      </c>
-      <c r="N10" t="s">
-        <v>20</v>
       </c>
       <c r="P10">
         <v>80</v>
@@ -913,13 +1001,13 @@
         <v>1</v>
       </c>
       <c r="L11" t="s">
+        <v>14</v>
+      </c>
+      <c r="M11" t="s">
         <v>16</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>18</v>
-      </c>
-      <c r="N11" t="s">
-        <v>20</v>
       </c>
       <c r="P11">
         <v>80</v>
@@ -960,13 +1048,13 @@
         <v>1</v>
       </c>
       <c r="L12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="M12" t="s">
+        <v>16</v>
+      </c>
+      <c r="N12" t="s">
         <v>18</v>
-      </c>
-      <c r="N12" t="s">
-        <v>20</v>
       </c>
       <c r="P12">
         <v>80</v>
@@ -977,4 +1065,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="3" max="3" width="17.25" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>2</v>
+      </c>
+      <c r="C10" t="s">
+        <v>36</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>